<commit_message>
initial iteration of build_seep. not working fully yet.
</commit_message>
<xml_diff>
--- a/inputs/slopes/input_template_lface3.xlsx
+++ b/inputs/slopes/input_template_lface3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/inputs/slopes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/CursorProjects/slopetools/inputs/slopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D56B4F9-B7C8-7B4D-8B73-C10DF9594A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CCC888-D251-834F-A937-23E2133D9B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31600" yWindow="500" windowWidth="35620" windowHeight="25080" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20140" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -3459,6 +3459,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>320</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3468,6 +3474,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3669,6 +3681,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3678,6 +3699,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4824,7 +4854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -5003,7 +5033,7 @@
   <dimension ref="B2:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5031,7 +5061,9 @@
       <c r="B3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="32">
+        <v>80</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>128</v>
       </c>
@@ -5062,16 +5094,24 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="3">
+        <v>320</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="3">
+        <v>320</v>
+      </c>
+      <c r="C6" s="3">
+        <v>80</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="3"/>
@@ -5140,16 +5180,28 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="3">
+        <v>115.7</v>
+      </c>
+      <c r="C17" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="3">
+        <v>170</v>
+      </c>
+      <c r="C18" s="3">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -5187,7 +5239,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5202,7 +5254,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H8"/>
+      <selection activeCell="G6" sqref="G6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5750,8 +5802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5900,11 +5952,21 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
+      <c r="R4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="V4" s="3">
+        <v>-1</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
@@ -5938,11 +6000,21 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
+      <c r="R5" s="3">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="V5" s="3">
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -5976,11 +6048,21 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
+      <c r="R6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="V6" s="3">
+        <v>-1</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="3">

</xml_diff>